<commit_message>
feat: CpiChartRepository.py 新增 绘制CPI 图表功能
</commit_message>
<xml_diff>
--- a/infrastructure/repository/data/CPI统计数据(2021~至今).xlsx
+++ b/infrastructure/repository/data/CPI统计数据(2021~至今).xlsx
@@ -425,242 +425,242 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>2021年1月</t>
+          <t>202101</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>2021年2月</t>
+          <t>202102</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>2021年3月</t>
+          <t>202103</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>2021年4月</t>
+          <t>202104</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>2021年5月</t>
+          <t>202105</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>2021年6月</t>
+          <t>202106</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>2021年7月</t>
+          <t>202107</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>2021年8月</t>
+          <t>202108</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>2021年9月</t>
+          <t>202109</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>2021年10月</t>
+          <t>202110</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>2021年11月</t>
+          <t>202111</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>2021年12月</t>
+          <t>202112</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>2022年1月</t>
+          <t>202201</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>2022年2月</t>
+          <t>202202</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>2022年3月</t>
+          <t>202203</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>2022年4月</t>
+          <t>202204</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>2022年5月</t>
+          <t>202205</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>2022年6月</t>
+          <t>202206</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>2022年7月</t>
+          <t>202207</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>2022年8月</t>
+          <t>202208</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>2022年9月</t>
+          <t>202209</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>2022年10月</t>
+          <t>202210</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>2022年11月</t>
+          <t>202211</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>2022年12月</t>
+          <t>202212</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>2023年1月</t>
+          <t>202301</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>2023年2月</t>
+          <t>202302</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>2023年3月</t>
+          <t>202303</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>2023年4月</t>
+          <t>202304</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>2023年5月</t>
+          <t>202305</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>2023年6月</t>
+          <t>202306</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>2023年7月</t>
+          <t>202307</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>2023年8月</t>
+          <t>202308</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>2023年9月</t>
+          <t>202309</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>2023年10月</t>
+          <t>202310</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>2023年11月</t>
+          <t>202311</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>2023年12月</t>
+          <t>202312</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>2024年1月</t>
+          <t>202401</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>2024年2月</t>
+          <t>202402</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>2024年3月</t>
+          <t>202403</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>2024年4月</t>
+          <t>202404</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>2024年5月</t>
+          <t>202405</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>2024年6月</t>
+          <t>202406</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>2024年7月</t>
+          <t>202407</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>2024年8月</t>
+          <t>202408</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>2024年9月</t>
+          <t>202409</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>2024年10月</t>
+          <t>202410</t>
         </is>
       </c>
       <c r="AV1" t="inlineStr">
         <is>
-          <t>2024年11月</t>
+          <t>202411</t>
         </is>
       </c>
       <c r="AW1" t="inlineStr">
         <is>
-          <t>2024年12月</t>
+          <t>202412</t>
         </is>
       </c>
     </row>

</xml_diff>